<commit_message>
Change df to long format
Added columns: lanes_open, operational_status and delay_minutes for standard lanes
</commit_message>
<xml_diff>
--- a/xls_files/rss-2025-03-28_16-04-56.xlsx
+++ b/xls_files/rss-2025-03-28_16-04-56.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\2 GitHub\BorderBuddy\xls_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F9CFC914-1D5D-4E35-808D-1EBFDD6D62B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29928848-262E-4A32-A17E-091CDB57BD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-21600" windowWidth="8055" windowHeight="20985" firstSheet="1" activeTab="1" xr2:uid="{94B302FC-273C-4C90-9679-43AB80C7914F}"/>
+    <workbookView xWindow="-105" yWindow="-21600" windowWidth="10215" windowHeight="20985" firstSheet="1" activeTab="1" xr2:uid="{94B302FC-273C-4C90-9679-43AB80C7914F}"/>
   </bookViews>
   <sheets>
     <sheet name="rss-2025-03-28_16-04-56" sheetId="1" r:id="rId1"/>
@@ -5101,7 +5101,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="44" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:42" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <v>230201</v>
       </c>
@@ -5751,7 +5751,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="51" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:42" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <v>240203</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:42" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <v>230402</v>
       </c>
@@ -6904,7 +6904,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:42" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <v>260401</v>
       </c>
@@ -7236,7 +7236,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:42" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <v>250601</v>
       </c>
@@ -8517,7 +8517,7 @@
   <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -8581,22 +8581,22 @@
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" t="s">
+      <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" t="s">
+      <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
     </row>
@@ -8626,22 +8626,22 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" t="s">
+      <c r="A22" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" t="s">
+      <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
+      <c r="A24" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -8691,22 +8691,22 @@
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
+      <c r="A34" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" t="s">
+      <c r="A35" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A36" t="s">
+      <c r="A36" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
+      <c r="A37" s="4" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>